<commit_message>
remove spaces from the report generated from transferReport.jrxml, returnedMaterials.jrxml, clientPartitions.jrxml, clientPayments.jrxml
</commit_message>
<xml_diff>
--- a/regionReport.xlsx
+++ b/regionReport.xlsx
@@ -200,7 +200,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1683693018" name="Picture">
+        <xdr:cNvPr id="381639883" name="Picture">
 </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
@@ -236,23 +236,24 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="1" width="3.3333333"/>
-    <col min="2" max="2" customWidth="1" width="0.33333334"/>
-    <col min="3" max="3" customWidth="1" width="13.5"/>
-    <col min="4" max="4" customWidth="1" width="9.5"/>
+    <col min="2" max="2" customWidth="1" width="0.16666667"/>
+    <col min="3" max="3" customWidth="1" width="14.833333"/>
+    <col min="4" max="4" customWidth="1" width="8.333333"/>
     <col min="5" max="5" customWidth="1" width="1.6666666"/>
-    <col min="6" max="6" customWidth="1" width="10.0"/>
-    <col min="7" max="7" customWidth="1" width="12.833333"/>
-    <col min="8" max="8" customWidth="1" width="8.833333"/>
-    <col min="9" max="9" customWidth="1" width="1.1666666"/>
-    <col min="10" max="10" customWidth="1" width="3.8333333"/>
-    <col min="11" max="11" customWidth="1" width="6.6666665"/>
-    <col min="12" max="12" customWidth="1" width="1.3333334"/>
-    <col min="13" max="13" customWidth="1" width="11.666667"/>
-    <col min="14" max="14" customWidth="1" width="0.33333334"/>
-    <col min="15" max="15" customWidth="1" width="5.0"/>
-    <col min="16" max="16" customWidth="1" width="5.6666665"/>
-    <col min="17" max="17" customWidth="1" width="2.6666667"/>
-    <col min="18" max="18" customWidth="1" width="0.8333333"/>
+    <col min="6" max="6" customWidth="1" width="6.3333335"/>
+    <col min="7" max="7" customWidth="1" width="0.6666667"/>
+    <col min="8" max="8" customWidth="1" width="17.166666"/>
+    <col min="9" max="9" customWidth="1" width="7.5"/>
+    <col min="10" max="10" customWidth="1" width="3.6666667"/>
+    <col min="11" max="11" customWidth="1" width="0.8333333"/>
+    <col min="12" max="12" customWidth="1" width="7.1666665"/>
+    <col min="13" max="13" customWidth="1" width="3.8333333"/>
+    <col min="14" max="14" customWidth="1" width="7.8333335"/>
+    <col min="15" max="15" customWidth="1" width="1.6666666"/>
+    <col min="16" max="16" customWidth="1" width="5.0"/>
+    <col min="17" max="17" customWidth="1" width="5.6666665"/>
+    <col min="18" max="18" customWidth="1" width="2.6666667"/>
+    <col min="19" max="19" customWidth="1" width="0.8333333"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" ht="22">
@@ -274,6 +275,7 @@
       <c r="P1" s="1" t="inlineStr"/>
       <c r="Q1" s="1" t="inlineStr"/>
       <c r="R1" s="1" t="inlineStr"/>
+      <c r="S1" s="1" t="inlineStr"/>
     </row>
     <row r="2" customHeight="1" ht="28">
       <c r="A2" s="1" t="inlineStr"/>
@@ -282,14 +284,14 @@
       <c r="D2" s="2" t="inlineStr"/>
       <c r="E2" s="1" t="inlineStr"/>
       <c r="F2" s="1" t="inlineStr"/>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">المواد المستلمة </t>
-          </r>
-        </is>
-      </c>
-      <c r="H2" s="3" t="inlineStr"/>
+      <c r="G2" s="1" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">النقل بين العملاء</t>
+          </r>
+        </is>
+      </c>
       <c r="I2" s="3" t="inlineStr"/>
       <c r="J2" s="3" t="inlineStr"/>
       <c r="K2" s="1" t="inlineStr"/>
@@ -300,6 +302,7 @@
       <c r="P2" s="1" t="inlineStr"/>
       <c r="Q2" s="1" t="inlineStr"/>
       <c r="R2" s="1" t="inlineStr"/>
+      <c r="S2" s="1" t="inlineStr"/>
     </row>
     <row r="3" customHeight="1" ht="2">
       <c r="A3" s="1" t="inlineStr"/>
@@ -320,6 +323,7 @@
       <c r="P3" s="1" t="inlineStr"/>
       <c r="Q3" s="1" t="inlineStr"/>
       <c r="R3" s="1" t="inlineStr"/>
+      <c r="S3" s="1" t="inlineStr"/>
     </row>
     <row r="4" customHeight="1" ht="20">
       <c r="A4" s="1" t="inlineStr"/>
@@ -330,7 +334,7 @@
       <c r="F4" s="4" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2024-01-02-2025-01-20</t>
+            <t xml:space="preserve">2024-08-13-2025-08-24</t>
           </r>
         </is>
       </c>
@@ -339,13 +343,14 @@
       <c r="I4" s="4" t="inlineStr"/>
       <c r="J4" s="4" t="inlineStr"/>
       <c r="K4" s="4" t="inlineStr"/>
-      <c r="L4" s="1" t="inlineStr"/>
+      <c r="L4" s="4" t="inlineStr"/>
       <c r="M4" s="1" t="inlineStr"/>
       <c r="N4" s="1" t="inlineStr"/>
       <c r="O4" s="1" t="inlineStr"/>
       <c r="P4" s="1" t="inlineStr"/>
       <c r="Q4" s="1" t="inlineStr"/>
       <c r="R4" s="1" t="inlineStr"/>
+      <c r="S4" s="1" t="inlineStr"/>
     </row>
     <row r="5" customHeight="1" ht="6">
       <c r="A5" s="1" t="inlineStr"/>
@@ -366,6 +371,7 @@
       <c r="P5" s="1" t="inlineStr"/>
       <c r="Q5" s="1" t="inlineStr"/>
       <c r="R5" s="1" t="inlineStr"/>
+      <c r="S5" s="1" t="inlineStr"/>
     </row>
     <row r="6" customHeight="1" ht="20">
       <c r="A6" s="1" t="inlineStr"/>
@@ -376,28 +382,29 @@
       <c r="F6" s="1" t="inlineStr"/>
       <c r="G6" s="1" t="inlineStr"/>
       <c r="H6" s="1" t="inlineStr"/>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">gas station 47</t>
-          </r>
-        </is>
-      </c>
-      <c r="J6" s="4" t="inlineStr"/>
+      <c r="I6" s="1" t="inlineStr"/>
+      <c r="J6" s="4" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">gas station 1</t>
+          </r>
+        </is>
+      </c>
       <c r="K6" s="4" t="inlineStr"/>
       <c r="L6" s="4" t="inlineStr"/>
       <c r="M6" s="4" t="inlineStr"/>
       <c r="N6" s="4" t="inlineStr"/>
-      <c r="O6" s="1" t="inlineStr"/>
-      <c r="P6" s="5" t="inlineStr">
+      <c r="O6" s="4" t="inlineStr"/>
+      <c r="P6" s="1" t="inlineStr"/>
+      <c r="Q6" s="5" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">الكازية</t>
           </r>
         </is>
       </c>
-      <c r="Q6" s="1" t="inlineStr"/>
       <c r="R6" s="1" t="inlineStr"/>
+      <c r="S6" s="1" t="inlineStr"/>
     </row>
     <row r="7" customHeight="1" ht="4">
       <c r="A7" s="1" t="inlineStr"/>
@@ -418,6 +425,7 @@
       <c r="P7" s="1" t="inlineStr"/>
       <c r="Q7" s="1" t="inlineStr"/>
       <c r="R7" s="1" t="inlineStr"/>
+      <c r="S7" s="1" t="inlineStr"/>
     </row>
     <row r="8" customHeight="1" ht="28">
       <c r="A8" s="1" t="inlineStr"/>
@@ -425,14 +433,14 @@
       <c r="C8" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">الاجمالي</t>
+            <t xml:space="preserve">الوجهة</t>
           </r>
         </is>
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">السعر</t>
+            <t xml:space="preserve">المصدر</t>
           </r>
         </is>
       </c>
@@ -441,65 +449,109 @@
       <c r="G8" s="6" t="inlineStr">
         <is>
           <r>
+            <t xml:space="preserve">الدفعة</t>
+          </r>
+        </is>
+      </c>
+      <c r="H8" s="6" t="inlineStr"/>
+      <c r="I8" s="6" t="inlineStr">
+        <is>
+          <r>
             <t xml:space="preserve">الكمية</t>
           </r>
         </is>
       </c>
-      <c r="H8" s="6" t="inlineStr">
+      <c r="J8" s="6" t="inlineStr"/>
+      <c r="K8" s="6" t="inlineStr"/>
+      <c r="L8" s="6" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">المادة</t>
           </r>
         </is>
       </c>
-      <c r="I8" s="6" t="inlineStr"/>
-      <c r="J8" s="6" t="inlineStr">
+      <c r="M8" s="6" t="inlineStr"/>
+      <c r="N8" s="6" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">المعرف</t>
           </r>
         </is>
       </c>
-      <c r="K8" s="6" t="inlineStr"/>
-      <c r="L8" s="6" t="inlineStr"/>
-      <c r="M8" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">المصدر</t>
-          </r>
-        </is>
-      </c>
-      <c r="N8" s="6" t="inlineStr">
+      <c r="O8" s="6" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">التاريخ</t>
           </r>
         </is>
       </c>
-      <c r="O8" s="6" t="inlineStr"/>
       <c r="P8" s="6" t="inlineStr"/>
       <c r="Q8" s="6" t="inlineStr"/>
-      <c r="R8" s="1" t="inlineStr"/>
-    </row>
-    <row r="9" customHeight="1" ht="6">
+      <c r="R8" s="6" t="inlineStr"/>
+      <c r="S8" s="1" t="inlineStr"/>
+    </row>
+    <row r="9" customHeight="1" ht="30">
       <c r="A9" s="1" t="inlineStr"/>
       <c r="B9" s="1" t="inlineStr"/>
-      <c r="C9" s="1" t="inlineStr"/>
-      <c r="D9" s="1" t="inlineStr"/>
-      <c r="E9" s="1" t="inlineStr"/>
-      <c r="F9" s="1" t="inlineStr"/>
-      <c r="G9" s="1" t="inlineStr"/>
-      <c r="H9" s="1" t="inlineStr"/>
-      <c r="I9" s="1" t="inlineStr"/>
-      <c r="J9" s="1" t="inlineStr"/>
-      <c r="K9" s="1" t="inlineStr"/>
-      <c r="L9" s="1" t="inlineStr"/>
-      <c r="M9" s="1" t="inlineStr"/>
-      <c r="N9" s="1" t="inlineStr"/>
-      <c r="O9" s="1" t="inlineStr"/>
-      <c r="P9" s="1" t="inlineStr"/>
-      <c r="Q9" s="1" t="inlineStr"/>
-      <c r="R9" s="1" t="inlineStr"/>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">gas station 2</t>
+          </r>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">gas station 1</t>
+          </r>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">100.0 USD</t>
+          </r>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">45000</t>
+          </r>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr"/>
+      <c r="K9" s="7" t="inlineStr"/>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">material 1</t>
+          </r>
+        </is>
+      </c>
+      <c r="M9" s="7" t="inlineStr"/>
+      <c r="N9" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">3</t>
+          </r>
+        </is>
+      </c>
+      <c r="O9" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2025-07-30T18:21:14</t>
+          </r>
+        </is>
+      </c>
+      <c r="P9" s="7" t="inlineStr"/>
+      <c r="Q9" s="7" t="inlineStr"/>
+      <c r="R9" s="7" t="inlineStr"/>
+      <c r="S9" s="1" t="inlineStr"/>
     </row>
     <row r="10" customHeight="1" ht="30">
       <c r="A10" s="1" t="inlineStr"/>
@@ -507,14 +559,14 @@
       <c r="C10" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">1250000.0</t>
+            <t xml:space="preserve">gas station 1</t>
           </r>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">500.0 SP</t>
+            <t xml:space="preserve">gas station 2</t>
           </r>
         </is>
       </c>
@@ -523,47 +575,48 @@
       <c r="G10" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2500</t>
-          </r>
-        </is>
-      </c>
-      <c r="H10" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">material 92</t>
-          </r>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2</t>
-          </r>
-        </is>
-      </c>
+            <t xml:space="preserve">100.0 USD</t>
+          </r>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">45000</t>
+          </r>
+        </is>
+      </c>
+      <c r="J10" s="7" t="inlineStr"/>
       <c r="K10" s="7" t="inlineStr"/>
-      <c r="L10" s="7" t="inlineStr"/>
-      <c r="M10" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref 39</t>
-          </r>
-        </is>
-      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">material 2</t>
+          </r>
+        </is>
+      </c>
+      <c r="M10" s="7" t="inlineStr"/>
       <c r="N10" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2024-12-01T16:12:34</t>
-          </r>
-        </is>
-      </c>
-      <c r="O10" s="7" t="inlineStr"/>
+            <t xml:space="preserve">4</t>
+          </r>
+        </is>
+      </c>
+      <c r="O10" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2025-07-30T18:21:14</t>
+          </r>
+        </is>
+      </c>
       <c r="P10" s="7" t="inlineStr"/>
       <c r="Q10" s="7" t="inlineStr"/>
-      <c r="R10" s="1" t="inlineStr"/>
-    </row>
-    <row r="11" customHeight="1" ht="6">
+      <c r="R10" s="7" t="inlineStr"/>
+      <c r="S10" s="1" t="inlineStr"/>
+    </row>
+    <row r="11" customHeight="1" ht="652">
       <c r="A11" s="1" t="inlineStr"/>
       <c r="B11" s="1" t="inlineStr"/>
       <c r="C11" s="1" t="inlineStr"/>
@@ -582,107 +635,29 @@
       <c r="P11" s="1" t="inlineStr"/>
       <c r="Q11" s="1" t="inlineStr"/>
       <c r="R11" s="1" t="inlineStr"/>
-    </row>
-    <row r="12" customHeight="1" ht="30">
-      <c r="A12" s="1" t="inlineStr"/>
-      <c r="B12" s="1" t="inlineStr"/>
-      <c r="C12" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">1250000.0</t>
-          </r>
-        </is>
-      </c>
-      <c r="D12" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">500.0 USD</t>
-          </r>
-        </is>
-      </c>
-      <c r="E12" s="7" t="inlineStr"/>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2500</t>
-          </r>
-        </is>
-      </c>
-      <c r="H12" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">material 92</t>
-          </r>
-        </is>
-      </c>
-      <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">1</t>
-          </r>
-        </is>
-      </c>
-      <c r="K12" s="7" t="inlineStr"/>
-      <c r="L12" s="7" t="inlineStr"/>
-      <c r="M12" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref 39</t>
-          </r>
-        </is>
-      </c>
-      <c r="N12" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2024-12-30T01:55:09</t>
-          </r>
-        </is>
-      </c>
-      <c r="O12" s="7" t="inlineStr"/>
-      <c r="P12" s="7" t="inlineStr"/>
-      <c r="Q12" s="7" t="inlineStr"/>
-      <c r="R12" s="1" t="inlineStr"/>
-    </row>
-    <row r="13" customHeight="1" ht="640">
-      <c r="A13" s="1" t="inlineStr"/>
-      <c r="B13" s="1" t="inlineStr"/>
-      <c r="C13" s="1" t="inlineStr"/>
-      <c r="D13" s="1" t="inlineStr"/>
-      <c r="E13" s="1" t="inlineStr"/>
-      <c r="F13" s="1" t="inlineStr"/>
-      <c r="G13" s="1" t="inlineStr"/>
-      <c r="H13" s="1" t="inlineStr"/>
-      <c r="I13" s="1" t="inlineStr"/>
-      <c r="J13" s="1" t="inlineStr"/>
-      <c r="K13" s="1" t="inlineStr"/>
-      <c r="L13" s="1" t="inlineStr"/>
-      <c r="M13" s="1" t="inlineStr"/>
-      <c r="N13" s="1" t="inlineStr"/>
-      <c r="O13" s="1" t="inlineStr"/>
-      <c r="P13" s="1" t="inlineStr"/>
-      <c r="Q13" s="1" t="inlineStr"/>
-      <c r="R13" s="1" t="inlineStr"/>
+      <c r="S11" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:D4"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="J6:O6"/>
     <mergeCell ref="D8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="O9:R9"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="O10:R10"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.00" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>